<commit_message>
Path Updated by Anuj Jain
</commit_message>
<xml_diff>
--- a/IPP_01/TestData/testdata.xlsx
+++ b/IPP_01/TestData/testdata.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5985"/>
+    <workbookView activeTab="1" windowHeight="5985" windowWidth="19320" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="1" r:id="rId2"/>
+    <sheet name="TestSuite" r:id="rId1" sheetId="2"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TestCases!$A$1:$J$898</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestSuite!$A$1:$C$36</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">TestCases!$A$1:$J$898</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">TestSuite!$A$1:$C$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8007" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8008" uniqueCount="687">
   <si>
     <t>S.No.</t>
   </si>
@@ -2067,22 +2067,26 @@
     <t>Registration Email Sent</t>
   </si>
   <si>
-    <t>C:\\Users\\jain.anuj\\workspace\\IPP_01\\AutoIT\\AutoDocumentUpload.exe</t>
-  </si>
-  <si>
     <t>C:\\Users\\jain.anuj\\workspace\\IPP_01\\AutoIT\\AutoUpload.exe</t>
   </si>
   <si>
-    <t>VC00001_10537</t>
-  </si>
-  <si>
     <t>VC00002_10538</t>
+  </si>
+  <si>
+    <t>VC00001_10587</t>
+  </si>
+  <si>
+    <t>C:\Users\jain.anuj\git\selenium\IPP_01\AutoIT\AutoDocumentUpload.exe</t>
+  </si>
+  <si>
+    <t>VC00001_10588</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2159,87 +2163,87 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="2" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2256,10 +2260,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2294,7 +2298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2329,7 +2333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2417,7 +2421,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -2426,13 +2430,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2442,7 +2446,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2451,7 +2455,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2460,7 +2464,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2470,12 +2474,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -2506,7 +2510,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -2525,7 +2529,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -2537,19 +2541,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="9" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="30.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2571,7 +2575,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2582,7 +2586,7 @@
         <v>416</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2593,7 +2597,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2604,7 +2608,7 @@
         <v>251</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2615,7 +2619,7 @@
         <v>252</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2626,7 +2630,7 @@
         <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2637,7 +2641,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2648,7 +2652,7 @@
         <v>415</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>284</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2769,7 +2773,7 @@
         <v>257</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2780,7 +2784,7 @@
         <v>258</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2791,7 +2795,7 @@
         <v>260</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2802,7 +2806,7 @@
         <v>259</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2813,7 +2817,7 @@
         <v>274</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2824,7 +2828,7 @@
         <v>275</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2835,7 +2839,7 @@
         <v>276</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2846,7 +2850,7 @@
         <v>278</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -3015,32 +3019,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J898"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K898"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="42.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="107.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="100.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="31.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="11" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="42.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="21.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="107.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="100.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="8.7109375" collapsed="true"/>
+    <col min="11" max="11" style="1" width="9.140625" collapsed="false"/>
+    <col min="12" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -5188,7 +5193,7 @@
         <v>6</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
@@ -5369,7 +5374,7 @@
       </c>
       <c r="F73" s="2" t="str">
         <f>J67</f>
-        <v>VC00001_10537</v>
+        <v>VC00001_10588</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>145</v>
@@ -6362,7 +6367,7 @@
         <v>6</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>6</v>
@@ -7561,7 +7566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
         <v>114</v>
       </c>
@@ -8587,7 +8592,7 @@
         <v>6</v>
       </c>
       <c r="J173" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
@@ -10016,7 +10021,7 @@
         <v>6</v>
       </c>
       <c r="F218" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G218" s="2" t="s">
         <v>6</v>
@@ -14826,7 +14831,7 @@
         <v>6</v>
       </c>
       <c r="F368" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G368" s="2" t="s">
         <v>6</v>
@@ -16301,7 +16306,7 @@
         <v>6</v>
       </c>
       <c r="F414" s="10" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G414" s="10" t="s">
         <v>6</v>
@@ -16813,9 +16818,9 @@
       <c r="F430" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G430" s="10">
+      <c r="G430" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H430" s="10" t="s">
         <v>6</v>
@@ -17422,9 +17427,9 @@
       <c r="F449" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G449" s="10">
+      <c r="G449" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H449" s="10" t="s">
         <v>6</v>
@@ -17532,7 +17537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="453" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="453" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A453" s="5" t="s">
         <v>183</v>
       </c>
@@ -17692,7 +17697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="458" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458" s="5" t="s">
         <v>183</v>
       </c>
@@ -18127,9 +18132,9 @@
       <c r="F471" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G471" s="10">
+      <c r="G471" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H471" s="10" t="s">
         <v>6</v>
@@ -19005,7 +19010,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="499" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A499" s="5" t="s">
         <v>196</v>
       </c>
@@ -19632,9 +19637,9 @@
       <c r="F518" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G518" s="10">
+      <c r="G518" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H518" s="10" t="s">
         <v>6</v>
@@ -21201,9 +21206,9 @@
       <c r="F567" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G567" s="10">
+      <c r="G567" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H567" s="10" t="s">
         <v>6</v>
@@ -22738,9 +22743,9 @@
       <c r="F615" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G615" s="10">
+      <c r="G615" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H615" s="10" t="s">
         <v>6</v>
@@ -24243,9 +24248,9 @@
       <c r="F662" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G662" s="10">
+      <c r="G662" s="10" t="n">
         <f>J429</f>
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="H662" s="10" t="s">
         <v>6</v>
@@ -26113,7 +26118,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="721" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="721" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A721" s="5" t="s">
         <v>441</v>
       </c>
@@ -28018,7 +28023,7 @@
         <v>6</v>
       </c>
       <c r="F780" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G780" s="2" t="s">
         <v>6</v>
@@ -29779,7 +29784,7 @@
         <v>6</v>
       </c>
       <c r="F835" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="G835" s="2" t="s">
         <v>6</v>
@@ -30421,7 +30426,7 @@
       </c>
       <c r="F855" s="28" t="str">
         <f>J67</f>
-        <v>VC00001_10537</v>
+        <v>VC00001_10588</v>
       </c>
       <c r="G855" s="24" t="s">
         <v>145</v>
@@ -31815,7 +31820,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>